<commit_message>
visual of country appeals for year w icons
</commit_message>
<xml_diff>
--- a/data/appealsData.xlsx
+++ b/data/appealsData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2049" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2234" uniqueCount="769">
   <si>
     <t>YEAR</t>
   </si>
@@ -2086,6 +2086,243 @@
   </si>
   <si>
     <t>terrorism</t>
+  </si>
+  <si>
+    <t>CATEGORY</t>
+  </si>
+  <si>
+    <t>cold</t>
+  </si>
+  <si>
+    <t>noidea</t>
+  </si>
+  <si>
+    <t>refugee</t>
+  </si>
+  <si>
+    <t>food</t>
+  </si>
+  <si>
+    <t>volcano</t>
+  </si>
+  <si>
+    <t>conflict</t>
+  </si>
+  <si>
+    <t>epidemic</t>
+  </si>
+  <si>
+    <t>landslides</t>
+  </si>
+  <si>
+    <t>populationmovement</t>
+  </si>
+  <si>
+    <t>typhoons</t>
+  </si>
+  <si>
+    <t>caprivifloods</t>
+  </si>
+  <si>
+    <t>solweziandmpulungufloods</t>
+  </si>
+  <si>
+    <t>humanitariancrisis</t>
+  </si>
+  <si>
+    <t>floodsandcyclone</t>
+  </si>
+  <si>
+    <t>cyclones</t>
+  </si>
+  <si>
+    <t>typhoonlekima</t>
+  </si>
+  <si>
+    <t>earthquaketsunami</t>
+  </si>
+  <si>
+    <t>flood</t>
+  </si>
+  <si>
+    <t>floodslandslides</t>
+  </si>
+  <si>
+    <t>cyclonesidr</t>
+  </si>
+  <si>
+    <t>cycloneguba</t>
+  </si>
+  <si>
+    <t>cycloneivan</t>
+  </si>
+  <si>
+    <t>coldwave</t>
+  </si>
+  <si>
+    <t>cyclonenargis</t>
+  </si>
+  <si>
+    <t>typhoonfengshen</t>
+  </si>
+  <si>
+    <t>foodsecurity</t>
+  </si>
+  <si>
+    <t>epidemics</t>
+  </si>
+  <si>
+    <t>foodinsecurity</t>
+  </si>
+  <si>
+    <t>hurricaneseason2008</t>
+  </si>
+  <si>
+    <t>floodsinghardaia</t>
+  </si>
+  <si>
+    <t>baluchistanearthquake</t>
+  </si>
+  <si>
+    <t>flashfloods</t>
+  </si>
+  <si>
+    <t>explosions</t>
+  </si>
+  <si>
+    <t>mudslidesandfloods</t>
+  </si>
+  <si>
+    <t>cycloneaila</t>
+  </si>
+  <si>
+    <t>westsumatraearthquake</t>
+  </si>
+  <si>
+    <t>khartoumstatefloods</t>
+  </si>
+  <si>
+    <t>thyphoons</t>
+  </si>
+  <si>
+    <t>floodsandtyphoons</t>
+  </si>
+  <si>
+    <t>earthquakeandtsunami</t>
+  </si>
+  <si>
+    <t>populationdisplacedfromiraq</t>
+  </si>
+  <si>
+    <t>severefoodshortages</t>
+  </si>
+  <si>
+    <t>severewinter</t>
+  </si>
+  <si>
+    <t>internallydisplacedpeople</t>
+  </si>
+  <si>
+    <t>supportforinternallydisplacedpeople</t>
+  </si>
+  <si>
+    <t>foodcrisis</t>
+  </si>
+  <si>
+    <t>yogyakartaearthquake</t>
+  </si>
+  <si>
+    <t>potentialdiarrhoeaoutbreak</t>
+  </si>
+  <si>
+    <t>tropicalstormagatha</t>
+  </si>
+  <si>
+    <t>moonsonfloods</t>
+  </si>
+  <si>
+    <t>javaeruptionsumatraearthquakeandtsunami</t>
+  </si>
+  <si>
+    <t>typhoonmegi</t>
+  </si>
+  <si>
+    <t>floodandcholera</t>
+  </si>
+  <si>
+    <t>preparednessforcivilunrest</t>
+  </si>
+  <si>
+    <t>floodsandlandslides</t>
+  </si>
+  <si>
+    <t>choleraoutbreak</t>
+  </si>
+  <si>
+    <t>monsoonfloods</t>
+  </si>
+  <si>
+    <t>complexemergency</t>
+  </si>
+  <si>
+    <t>floods2011</t>
+  </si>
+  <si>
+    <t>droughtandfoodinsecurity</t>
+  </si>
+  <si>
+    <t>tropicalstormwashi</t>
+  </si>
+  <si>
+    <t>earthquakeedan</t>
+  </si>
+  <si>
+    <t>foodemergency</t>
+  </si>
+  <si>
+    <t>tornado</t>
+  </si>
+  <si>
+    <t>explosionofammunitiondepot</t>
+  </si>
+  <si>
+    <t>mudslides</t>
+  </si>
+  <si>
+    <t>flooding</t>
+  </si>
+  <si>
+    <t>palestinianrefugees</t>
+  </si>
+  <si>
+    <t>fire</t>
+  </si>
+  <si>
+    <t>peoplefleeingburndi</t>
+  </si>
+  <si>
+    <t>snowfalls</t>
+  </si>
+  <si>
+    <t>centralafricanrefugees</t>
+  </si>
+  <si>
+    <t>doroudearthquake</t>
+  </si>
+  <si>
+    <t>watersanitation</t>
+  </si>
+  <si>
+    <t>youthalliance</t>
+  </si>
+  <si>
+    <t>tropicalstormadrian</t>
+  </si>
+  <si>
+    <t>avianflu</t>
+  </si>
+  <si>
+    <t>avianfluawarenesscampaign</t>
   </si>
 </sst>
 </file>
@@ -2614,13 +2851,16 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2985,14 +3225,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I172" sqref="I172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="59.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="22" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1"/>
     <col min="5" max="6" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
@@ -3030,6 +3270,9 @@
       <c r="H1" s="1" t="s">
         <v>365</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>690</v>
+      </c>
       <c r="J1" s="1" t="s">
         <v>364</v>
       </c>
@@ -3847,6 +4090,9 @@
       <c r="H21" s="1" t="s">
         <v>276</v>
       </c>
+      <c r="I21" s="1" t="s">
+        <v>691</v>
+      </c>
       <c r="J21" s="1" t="s">
         <v>24</v>
       </c>
@@ -3885,6 +4131,9 @@
       <c r="H22" s="1" t="s">
         <v>318</v>
       </c>
+      <c r="I22" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J22" s="1" t="s">
         <v>6</v>
       </c>
@@ -3923,6 +4172,9 @@
       <c r="H23" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I23" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J23" s="1" t="s">
         <v>6</v>
       </c>
@@ -3961,6 +4213,9 @@
       <c r="H24" s="1" t="s">
         <v>290</v>
       </c>
+      <c r="I24" s="4" t="s">
+        <v>692</v>
+      </c>
       <c r="J24" s="1" t="s">
         <v>13</v>
       </c>
@@ -3999,6 +4254,9 @@
       <c r="H25" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I25" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J25" s="1" t="s">
         <v>6</v>
       </c>
@@ -4037,6 +4295,9 @@
       <c r="H26" s="1" t="s">
         <v>278</v>
       </c>
+      <c r="I26" s="1" t="s">
+        <v>693</v>
+      </c>
       <c r="J26" s="1" t="s">
         <v>13</v>
       </c>
@@ -4075,6 +4336,9 @@
       <c r="H27" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I27" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J27" s="1" t="s">
         <v>6</v>
       </c>
@@ -4113,6 +4377,9 @@
       <c r="H28" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I28" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J28" s="1" t="s">
         <v>6</v>
       </c>
@@ -4151,6 +4418,9 @@
       <c r="H29" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="I29" s="1" t="s">
+        <v>694</v>
+      </c>
       <c r="J29" s="1" t="s">
         <v>13</v>
       </c>
@@ -4189,6 +4459,9 @@
       <c r="H30" s="1" t="s">
         <v>299</v>
       </c>
+      <c r="I30" s="4" t="s">
+        <v>692</v>
+      </c>
       <c r="J30" s="1" t="s">
         <v>13</v>
       </c>
@@ -4227,6 +4500,9 @@
       <c r="H31" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="I31" s="1" t="s">
+        <v>694</v>
+      </c>
       <c r="J31" s="1" t="s">
         <v>13</v>
       </c>
@@ -4259,6 +4535,9 @@
       <c r="H32" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="I32" s="1" t="s">
+        <v>694</v>
+      </c>
       <c r="J32" s="1" t="s">
         <v>13</v>
       </c>
@@ -4291,6 +4570,9 @@
       <c r="H33" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="I33" s="1" t="s">
+        <v>694</v>
+      </c>
       <c r="J33" s="1" t="s">
         <v>13</v>
       </c>
@@ -4323,6 +4605,9 @@
       <c r="H34" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="I34" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J34" s="1" t="s">
         <v>6</v>
       </c>
@@ -4361,6 +4646,9 @@
       <c r="H35" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="I35" s="1" t="s">
+        <v>694</v>
+      </c>
       <c r="J35" s="1" t="s">
         <v>13</v>
       </c>
@@ -4399,6 +4687,9 @@
       <c r="H36" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="I36" s="1" t="s">
+        <v>694</v>
+      </c>
       <c r="J36" s="1" t="s">
         <v>13</v>
       </c>
@@ -4431,6 +4722,9 @@
       <c r="H37" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="I37" s="1" t="s">
+        <v>686</v>
+      </c>
       <c r="J37" s="1" t="s">
         <v>42</v>
       </c>
@@ -4469,6 +4763,9 @@
       <c r="H38" s="1" t="s">
         <v>284</v>
       </c>
+      <c r="I38" s="1" t="s">
+        <v>695</v>
+      </c>
       <c r="J38" s="1" t="s">
         <v>285</v>
       </c>
@@ -4507,6 +4804,9 @@
       <c r="H39" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="I39" s="1" t="s">
+        <v>694</v>
+      </c>
       <c r="J39" s="1" t="s">
         <v>13</v>
       </c>
@@ -4539,6 +4839,9 @@
       <c r="H40" s="1" t="s">
         <v>298</v>
       </c>
+      <c r="I40" s="1" t="s">
+        <v>687</v>
+      </c>
       <c r="J40" s="1" t="s">
         <v>2</v>
       </c>
@@ -4577,6 +4880,9 @@
       <c r="H41" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="I41" s="1" t="s">
+        <v>694</v>
+      </c>
       <c r="J41" s="1" t="s">
         <v>13</v>
       </c>
@@ -4609,6 +4915,9 @@
       <c r="H42" s="1" t="s">
         <v>289</v>
       </c>
+      <c r="I42" s="1" t="s">
+        <v>696</v>
+      </c>
       <c r="J42" s="1" t="s">
         <v>13</v>
       </c>
@@ -4647,6 +4956,9 @@
       <c r="H43" s="1" t="s">
         <v>316</v>
       </c>
+      <c r="I43" s="1" t="s">
+        <v>693</v>
+      </c>
       <c r="J43" s="1" t="s">
         <v>13</v>
       </c>
@@ -4685,6 +4997,9 @@
       <c r="H44" s="1" t="s">
         <v>259</v>
       </c>
+      <c r="I44" s="1" t="s">
+        <v>693</v>
+      </c>
       <c r="J44" s="1" t="s">
         <v>13</v>
       </c>
@@ -4723,6 +5038,9 @@
       <c r="H45" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="I45" s="1" t="s">
+        <v>685</v>
+      </c>
       <c r="J45" s="1" t="s">
         <v>6</v>
       </c>
@@ -4761,6 +5079,9 @@
       <c r="H46" s="1" t="s">
         <v>261</v>
       </c>
+      <c r="I46" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J46" s="1" t="s">
         <v>6</v>
       </c>
@@ -4799,6 +5120,9 @@
       <c r="H47" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="I47" s="1" t="s">
+        <v>685</v>
+      </c>
       <c r="J47" s="1" t="s">
         <v>24</v>
       </c>
@@ -4837,6 +5161,9 @@
       <c r="H48" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="I48" s="1" t="s">
+        <v>697</v>
+      </c>
       <c r="J48" s="1" t="s">
         <v>71</v>
       </c>
@@ -4875,6 +5202,9 @@
       <c r="H49" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I49" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J49" s="1" t="s">
         <v>6</v>
       </c>
@@ -4913,6 +5243,9 @@
       <c r="H50" s="1" t="s">
         <v>266</v>
       </c>
+      <c r="I50" s="1" t="s">
+        <v>698</v>
+      </c>
       <c r="J50" s="1" t="s">
         <v>6</v>
       </c>
@@ -4951,6 +5284,9 @@
       <c r="H51" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="I51" s="1" t="s">
+        <v>685</v>
+      </c>
       <c r="J51" s="1" t="s">
         <v>24</v>
       </c>
@@ -4989,6 +5325,9 @@
       <c r="H52" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="I52" s="1" t="s">
+        <v>685</v>
+      </c>
       <c r="J52" s="1" t="s">
         <v>24</v>
       </c>
@@ -5027,6 +5366,9 @@
       <c r="H53" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="I53" s="1" t="s">
+        <v>697</v>
+      </c>
       <c r="J53" s="1" t="s">
         <v>71</v>
       </c>
@@ -5065,6 +5407,9 @@
       <c r="H54" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="I54" s="1" t="s">
+        <v>686</v>
+      </c>
       <c r="J54" s="1" t="s">
         <v>42</v>
       </c>
@@ -5103,6 +5448,9 @@
       <c r="H55" s="1" t="s">
         <v>264</v>
       </c>
+      <c r="I55" s="4" t="s">
+        <v>692</v>
+      </c>
       <c r="J55" s="1" t="s">
         <v>71</v>
       </c>
@@ -5141,6 +5489,9 @@
       <c r="H56" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I56" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J56" s="1" t="s">
         <v>6</v>
       </c>
@@ -5179,6 +5530,9 @@
       <c r="H57" s="1" t="s">
         <v>132</v>
       </c>
+      <c r="I57" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J57" s="1" t="s">
         <v>6</v>
       </c>
@@ -5217,6 +5571,9 @@
       <c r="H58" s="1" t="s">
         <v>224</v>
       </c>
+      <c r="I58" s="1" t="s">
+        <v>695</v>
+      </c>
       <c r="J58" s="1" t="s">
         <v>42</v>
       </c>
@@ -5255,6 +5612,9 @@
       <c r="H59" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I59" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J59" s="1" t="s">
         <v>6</v>
       </c>
@@ -5293,6 +5653,9 @@
       <c r="H60" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I60" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J60" s="1" t="s">
         <v>6</v>
       </c>
@@ -5331,6 +5694,9 @@
       <c r="H61" s="1" t="s">
         <v>265</v>
       </c>
+      <c r="I61" s="1" t="s">
+        <v>687</v>
+      </c>
       <c r="J61" s="1" t="s">
         <v>2</v>
       </c>
@@ -5369,6 +5735,9 @@
       <c r="H62" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="I62" s="1" t="s">
+        <v>699</v>
+      </c>
       <c r="J62" s="1" t="s">
         <v>13</v>
       </c>
@@ -5407,6 +5776,9 @@
       <c r="H63" s="1" t="s">
         <v>265</v>
       </c>
+      <c r="I63" s="1" t="s">
+        <v>700</v>
+      </c>
       <c r="J63" s="1" t="s">
         <v>6</v>
       </c>
@@ -5445,6 +5817,9 @@
       <c r="H64" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I64" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J64" s="1" t="s">
         <v>6</v>
       </c>
@@ -5483,6 +5858,9 @@
       <c r="H65" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I65" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J65" s="1" t="s">
         <v>6</v>
       </c>
@@ -5521,6 +5899,9 @@
       <c r="H66" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="I66" s="1" t="s">
+        <v>686</v>
+      </c>
       <c r="J66" s="1" t="s">
         <v>6</v>
       </c>
@@ -5559,6 +5940,9 @@
       <c r="H67" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I67" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J67" s="1" t="s">
         <v>6</v>
       </c>
@@ -5597,6 +5981,9 @@
       <c r="H68" s="1" t="s">
         <v>239</v>
       </c>
+      <c r="I68" s="1" t="s">
+        <v>701</v>
+      </c>
       <c r="J68" s="1" t="s">
         <v>6</v>
       </c>
@@ -5635,6 +6022,9 @@
       <c r="H69" s="1" t="s">
         <v>256</v>
       </c>
+      <c r="I69" s="1" t="s">
+        <v>702</v>
+      </c>
       <c r="J69" s="1" t="s">
         <v>6</v>
       </c>
@@ -5673,6 +6063,9 @@
       <c r="H70" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I70" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J70" s="1" t="s">
         <v>6</v>
       </c>
@@ -5711,6 +6104,9 @@
       <c r="H71" s="1" t="s">
         <v>234</v>
       </c>
+      <c r="I71" s="1" t="s">
+        <v>703</v>
+      </c>
       <c r="J71" s="1" t="s">
         <v>13</v>
       </c>
@@ -5749,6 +6145,9 @@
       <c r="H72" s="1" t="s">
         <v>238</v>
       </c>
+      <c r="I72" s="1" t="s">
+        <v>704</v>
+      </c>
       <c r="J72" s="1" t="s">
         <v>27</v>
       </c>
@@ -5787,6 +6186,9 @@
       <c r="H73" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I73" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J73" s="1" t="s">
         <v>6</v>
       </c>
@@ -5825,6 +6227,9 @@
       <c r="H74" s="1" t="s">
         <v>235</v>
       </c>
+      <c r="I74" s="1" t="s">
+        <v>705</v>
+      </c>
       <c r="J74" s="1" t="s">
         <v>2</v>
       </c>
@@ -5863,6 +6268,9 @@
       <c r="H75" s="1" t="s">
         <v>254</v>
       </c>
+      <c r="I75" s="1" t="s">
+        <v>706</v>
+      </c>
       <c r="J75" s="1" t="s">
         <v>2</v>
       </c>
@@ -5901,6 +6309,9 @@
       <c r="H76" s="1" t="s">
         <v>247</v>
       </c>
+      <c r="I76" s="1" t="s">
+        <v>707</v>
+      </c>
       <c r="J76" s="1" t="s">
         <v>42</v>
       </c>
@@ -5939,6 +6350,9 @@
       <c r="H77" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I77" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J77" s="1" t="s">
         <v>6</v>
       </c>
@@ -5977,6 +6391,9 @@
       <c r="H78" s="1" t="s">
         <v>132</v>
       </c>
+      <c r="I78" s="1" t="s">
+        <v>708</v>
+      </c>
       <c r="J78" s="1" t="s">
         <v>6</v>
       </c>
@@ -6015,6 +6432,9 @@
       <c r="H79" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I79" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J79" s="1" t="s">
         <v>6</v>
       </c>
@@ -6053,6 +6473,9 @@
       <c r="H80" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="I80" s="1" t="s">
+        <v>686</v>
+      </c>
       <c r="J80" s="1" t="s">
         <v>42</v>
       </c>
@@ -6091,6 +6514,9 @@
       <c r="H81" s="1" t="s">
         <v>240</v>
       </c>
+      <c r="I81" s="1" t="s">
+        <v>709</v>
+      </c>
       <c r="J81" s="1" t="s">
         <v>6</v>
       </c>
@@ -6129,6 +6555,9 @@
       <c r="H82" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I82" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J82" s="1" t="s">
         <v>6</v>
       </c>
@@ -6167,6 +6596,9 @@
       <c r="H83" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I83" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J83" s="1" t="s">
         <v>6</v>
       </c>
@@ -6205,6 +6637,9 @@
       <c r="H84" s="1" t="s">
         <v>228</v>
       </c>
+      <c r="I84" s="1" t="s">
+        <v>710</v>
+      </c>
       <c r="J84" s="1" t="s">
         <v>2</v>
       </c>
@@ -6243,6 +6678,9 @@
       <c r="H85" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I85" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J85" s="1" t="s">
         <v>6</v>
       </c>
@@ -6281,6 +6719,9 @@
       <c r="H86" s="1" t="s">
         <v>243</v>
       </c>
+      <c r="I86" s="1" t="s">
+        <v>711</v>
+      </c>
       <c r="J86" s="1" t="s">
         <v>2</v>
       </c>
@@ -6319,6 +6760,9 @@
       <c r="H87" s="1" t="s">
         <v>215</v>
       </c>
+      <c r="I87" s="1" t="s">
+        <v>703</v>
+      </c>
       <c r="J87" s="1" t="s">
         <v>13</v>
       </c>
@@ -6357,6 +6801,9 @@
       <c r="H88" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="I88" s="1" t="s">
+        <v>699</v>
+      </c>
       <c r="J88" s="1" t="s">
         <v>13</v>
       </c>
@@ -6395,6 +6842,9 @@
       <c r="H89" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="I89" s="1" t="s">
+        <v>712</v>
+      </c>
       <c r="J89" s="1" t="s">
         <v>2</v>
       </c>
@@ -6433,6 +6883,9 @@
       <c r="H90" s="1" t="s">
         <v>193</v>
       </c>
+      <c r="I90" s="1" t="s">
+        <v>713</v>
+      </c>
       <c r="J90" s="1" t="s">
         <v>24</v>
       </c>
@@ -6471,6 +6924,9 @@
       <c r="H91" s="1" t="s">
         <v>218</v>
       </c>
+      <c r="I91" s="1" t="s">
+        <v>686</v>
+      </c>
       <c r="J91" s="1" t="s">
         <v>42</v>
       </c>
@@ -6509,6 +6965,9 @@
       <c r="H92" s="1" t="s">
         <v>217</v>
       </c>
+      <c r="I92" s="1" t="s">
+        <v>714</v>
+      </c>
       <c r="J92" s="1" t="s">
         <v>2</v>
       </c>
@@ -6547,6 +7006,9 @@
       <c r="H93" s="1" t="s">
         <v>198</v>
       </c>
+      <c r="I93" s="1" t="s">
+        <v>715</v>
+      </c>
       <c r="J93" s="1" t="s">
         <v>2</v>
       </c>
@@ -6585,6 +7047,9 @@
       <c r="H94" s="1" t="s">
         <v>212</v>
       </c>
+      <c r="I94" s="1" t="s">
+        <v>716</v>
+      </c>
       <c r="J94" s="1" t="s">
         <v>13</v>
       </c>
@@ -6623,6 +7088,9 @@
       <c r="H95" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I95" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J95" s="1" t="s">
         <v>6</v>
       </c>
@@ -6661,6 +7129,9 @@
       <c r="H96" s="1" t="s">
         <v>216</v>
       </c>
+      <c r="I96" s="1" t="s">
+        <v>717</v>
+      </c>
       <c r="J96" s="1" t="s">
         <v>71</v>
       </c>
@@ -6699,6 +7170,9 @@
       <c r="H97" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="I97" s="1" t="s">
+        <v>718</v>
+      </c>
       <c r="J97" s="1" t="s">
         <v>13</v>
       </c>
@@ -6737,6 +7211,9 @@
       <c r="H98" s="1" t="s">
         <v>203</v>
       </c>
+      <c r="I98" s="1" t="s">
+        <v>719</v>
+      </c>
       <c r="J98" s="1" t="s">
         <v>2</v>
       </c>
@@ -6775,6 +7252,9 @@
       <c r="H99" s="1" t="s">
         <v>203</v>
       </c>
+      <c r="I99" s="1" t="s">
+        <v>719</v>
+      </c>
       <c r="J99" s="1" t="s">
         <v>2</v>
       </c>
@@ -6813,6 +7293,9 @@
       <c r="H100" s="1" t="s">
         <v>201</v>
       </c>
+      <c r="I100" s="1" t="s">
+        <v>720</v>
+      </c>
       <c r="J100" s="1" t="s">
         <v>6</v>
       </c>
@@ -6851,6 +7334,9 @@
       <c r="H101" s="1" t="s">
         <v>179</v>
       </c>
+      <c r="I101" s="1" t="s">
+        <v>721</v>
+      </c>
       <c r="J101" s="1" t="s">
         <v>6</v>
       </c>
@@ -6889,6 +7375,9 @@
       <c r="H102" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="I102" s="1" t="s">
+        <v>722</v>
+      </c>
       <c r="J102" s="1" t="s">
         <v>6</v>
       </c>
@@ -6927,6 +7416,9 @@
       <c r="H103" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I103" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J103" s="1" t="s">
         <v>6</v>
       </c>
@@ -6965,6 +7457,9 @@
       <c r="H104" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I104" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J104" s="1" t="s">
         <v>6</v>
       </c>
@@ -7003,6 +7498,9 @@
       <c r="H105" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="I105" s="1" t="s">
+        <v>699</v>
+      </c>
       <c r="J105" s="1" t="s">
         <v>13</v>
       </c>
@@ -7041,6 +7539,9 @@
       <c r="H106" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I106" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J106" s="1" t="s">
         <v>6</v>
       </c>
@@ -7079,6 +7580,9 @@
       <c r="H107" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I107" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J107" s="1" t="s">
         <v>6</v>
       </c>
@@ -7117,6 +7621,9 @@
       <c r="H108" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I108" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J108" s="1" t="s">
         <v>6</v>
       </c>
@@ -7155,6 +7662,9 @@
       <c r="H109" s="1" t="s">
         <v>173</v>
       </c>
+      <c r="I109" s="1" t="s">
+        <v>723</v>
+      </c>
       <c r="J109" s="1" t="s">
         <v>15</v>
       </c>
@@ -7193,6 +7703,9 @@
       <c r="H110" s="1" t="s">
         <v>167</v>
       </c>
+      <c r="I110" s="1" t="s">
+        <v>724</v>
+      </c>
       <c r="J110" s="1" t="s">
         <v>6</v>
       </c>
@@ -7231,6 +7744,9 @@
       <c r="H111" s="1" t="s">
         <v>185</v>
       </c>
+      <c r="I111" s="1" t="s">
+        <v>725</v>
+      </c>
       <c r="J111" s="1" t="s">
         <v>2</v>
       </c>
@@ -7269,6 +7785,9 @@
       <c r="H112" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I112" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J112" s="1" t="s">
         <v>6</v>
       </c>
@@ -7307,6 +7826,9 @@
       <c r="H113" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="I113" s="1" t="s">
+        <v>685</v>
+      </c>
       <c r="J113" s="1" t="s">
         <v>24</v>
       </c>
@@ -7345,6 +7867,9 @@
       <c r="H114" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I114" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J114" s="1" t="s">
         <v>6</v>
       </c>
@@ -7383,6 +7908,9 @@
       <c r="H115" s="1" t="s">
         <v>184</v>
       </c>
+      <c r="I115" s="1" t="s">
+        <v>726</v>
+      </c>
       <c r="J115" s="1" t="s">
         <v>42</v>
       </c>
@@ -7421,6 +7949,9 @@
       <c r="H116" s="1" t="s">
         <v>182</v>
       </c>
+      <c r="I116" s="1" t="s">
+        <v>727</v>
+      </c>
       <c r="J116" s="1" t="s">
         <v>71</v>
       </c>
@@ -7459,6 +7990,9 @@
       <c r="H117" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I117" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J117" s="1" t="s">
         <v>6</v>
       </c>
@@ -7497,6 +8031,9 @@
       <c r="H118" s="1" t="s">
         <v>186</v>
       </c>
+      <c r="I118" s="1" t="s">
+        <v>728</v>
+      </c>
       <c r="J118" s="1" t="s">
         <v>2</v>
       </c>
@@ -7535,6 +8072,9 @@
       <c r="H119" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="I119" s="1" t="s">
+        <v>729</v>
+      </c>
       <c r="J119" s="1" t="s">
         <v>27</v>
       </c>
@@ -7573,6 +8113,9 @@
       <c r="H120" s="1" t="s">
         <v>169</v>
       </c>
+      <c r="I120" s="1" t="s">
+        <v>730</v>
+      </c>
       <c r="J120" s="1" t="s">
         <v>42</v>
       </c>
@@ -7611,6 +8154,9 @@
       <c r="H121" s="1" t="s">
         <v>179</v>
       </c>
+      <c r="I121" s="1" t="s">
+        <v>721</v>
+      </c>
       <c r="J121" s="1" t="s">
         <v>42</v>
       </c>
@@ -7649,6 +8195,9 @@
       <c r="H122" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I122" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J122" s="1" t="s">
         <v>196</v>
       </c>
@@ -7687,6 +8236,9 @@
       <c r="H123" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="I123" s="1" t="s">
+        <v>686</v>
+      </c>
       <c r="J123" s="1" t="s">
         <v>42</v>
       </c>
@@ -7725,6 +8277,9 @@
       <c r="H124" s="1" t="s">
         <v>161</v>
       </c>
+      <c r="I124" s="1" t="s">
+        <v>731</v>
+      </c>
       <c r="J124" s="1" t="s">
         <v>13</v>
       </c>
@@ -7763,6 +8318,9 @@
       <c r="H125" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I125" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J125" s="1" t="s">
         <v>6</v>
       </c>
@@ -7801,6 +8359,9 @@
       <c r="H126" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="I126" s="1" t="s">
+        <v>686</v>
+      </c>
       <c r="J126" s="1" t="s">
         <v>42</v>
       </c>
@@ -7839,6 +8400,9 @@
       <c r="H127" s="1" t="s">
         <v>140</v>
       </c>
+      <c r="I127" s="1" t="s">
+        <v>732</v>
+      </c>
       <c r="J127" s="1" t="s">
         <v>13</v>
       </c>
@@ -7877,6 +8441,9 @@
       <c r="H128" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="I128" s="1" t="s">
+        <v>685</v>
+      </c>
       <c r="J128" s="1" t="s">
         <v>24</v>
       </c>
@@ -7915,6 +8482,9 @@
       <c r="H129" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="I129" s="1" t="s">
+        <v>733</v>
+      </c>
       <c r="J129" s="1" t="s">
         <v>24</v>
       </c>
@@ -7953,6 +8523,9 @@
       <c r="H130" s="1" t="s">
         <v>121</v>
       </c>
+      <c r="I130" s="1" t="s">
+        <v>718</v>
+      </c>
       <c r="J130" s="1" t="s">
         <v>13</v>
       </c>
@@ -7991,6 +8564,9 @@
       <c r="H131" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="I131" s="1" t="s">
+        <v>734</v>
+      </c>
       <c r="J131" s="1" t="s">
         <v>13</v>
       </c>
@@ -8029,6 +8605,9 @@
       <c r="H132" s="1" t="s">
         <v>141</v>
       </c>
+      <c r="I132" s="1" t="s">
+        <v>735</v>
+      </c>
       <c r="J132" s="1" t="s">
         <v>13</v>
       </c>
@@ -8067,6 +8646,9 @@
       <c r="H133" s="1" t="s">
         <v>154</v>
       </c>
+      <c r="I133" s="1" t="s">
+        <v>736</v>
+      </c>
       <c r="J133" s="1" t="s">
         <v>13</v>
       </c>
@@ -8105,6 +8687,9 @@
       <c r="H134" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="I134" s="1" t="s">
+        <v>737</v>
+      </c>
       <c r="J134" s="1" t="s">
         <v>42</v>
       </c>
@@ -8143,6 +8728,9 @@
       <c r="H135" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I135" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J135" s="1" t="s">
         <v>6</v>
       </c>
@@ -8181,6 +8769,9 @@
       <c r="H136" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="I136" s="1" t="s">
+        <v>738</v>
+      </c>
       <c r="J136" s="1" t="s">
         <v>71</v>
       </c>
@@ -8219,6 +8810,9 @@
       <c r="H137" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="I137" s="1" t="s">
+        <v>739</v>
+      </c>
       <c r="J137" s="1" t="s">
         <v>2</v>
       </c>
@@ -8257,6 +8851,9 @@
       <c r="H138" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="I138" s="1" t="s">
+        <v>688</v>
+      </c>
       <c r="J138" s="1" t="s">
         <v>13</v>
       </c>
@@ -8295,6 +8892,9 @@
       <c r="H139" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="I139" s="1" t="s">
+        <v>699</v>
+      </c>
       <c r="J139" s="1" t="s">
         <v>13</v>
       </c>
@@ -8333,6 +8933,9 @@
       <c r="H140" s="1" t="s">
         <v>159</v>
       </c>
+      <c r="I140" s="1" t="s">
+        <v>740</v>
+      </c>
       <c r="J140" s="1" t="s">
         <v>6</v>
       </c>
@@ -8371,6 +8974,9 @@
       <c r="H141" s="1" t="s">
         <v>123</v>
       </c>
+      <c r="I141" s="1" t="s">
+        <v>741</v>
+      </c>
       <c r="J141" s="1" t="s">
         <v>42</v>
       </c>
@@ -8409,6 +9015,9 @@
       <c r="H142" s="1" t="s">
         <v>120</v>
       </c>
+      <c r="I142" s="1" t="s">
+        <v>742</v>
+      </c>
       <c r="J142" s="1" t="s">
         <v>2</v>
       </c>
@@ -8447,6 +9056,9 @@
       <c r="H143" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I143" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J143" s="1" t="s">
         <v>6</v>
       </c>
@@ -8485,6 +9097,9 @@
       <c r="H144" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="I144" s="1" t="s">
+        <v>743</v>
+      </c>
       <c r="J144" s="1" t="s">
         <v>69</v>
       </c>
@@ -8523,6 +9138,9 @@
       <c r="H145" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I145" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J145" s="1" t="s">
         <v>6</v>
       </c>
@@ -8561,6 +9179,9 @@
       <c r="H146" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I146" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J146" s="1" t="s">
         <v>6</v>
       </c>
@@ -8599,6 +9220,9 @@
       <c r="H147" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I147" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J147" s="1" t="s">
         <v>6</v>
       </c>
@@ -8637,6 +9261,9 @@
       <c r="H148" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="I148" s="1" t="s">
+        <v>686</v>
+      </c>
       <c r="J148" s="1" t="s">
         <v>42</v>
       </c>
@@ -8675,6 +9302,9 @@
       <c r="H149" s="1" t="s">
         <v>118</v>
       </c>
+      <c r="I149" s="1" t="s">
+        <v>744</v>
+      </c>
       <c r="J149" s="1" t="s">
         <v>13</v>
       </c>
@@ -8713,6 +9343,9 @@
       <c r="H150" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I150" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J150" s="1" t="s">
         <v>6</v>
       </c>
@@ -8751,6 +9384,9 @@
       <c r="H151" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="I151" s="1" t="s">
+        <v>685</v>
+      </c>
       <c r="J151" s="1" t="s">
         <v>24</v>
       </c>
@@ -8789,6 +9425,9 @@
       <c r="H152" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="I152" s="1" t="s">
+        <v>745</v>
+      </c>
       <c r="J152" s="1" t="s">
         <v>6</v>
       </c>
@@ -8827,6 +9466,9 @@
       <c r="H153" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="I153" s="1" t="s">
+        <v>699</v>
+      </c>
       <c r="J153" s="1" t="s">
         <v>13</v>
       </c>
@@ -8865,6 +9507,9 @@
       <c r="H154" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="I154" s="1" t="s">
+        <v>746</v>
+      </c>
       <c r="J154" s="1" t="s">
         <v>71</v>
       </c>
@@ -8903,6 +9548,9 @@
       <c r="H155" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I155" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J155" s="1" t="s">
         <v>6</v>
       </c>
@@ -8941,6 +9589,9 @@
       <c r="H156" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="I156" s="1" t="s">
+        <v>747</v>
+      </c>
       <c r="J156" s="1" t="s">
         <v>6</v>
       </c>
@@ -8979,6 +9630,9 @@
       <c r="H157" s="1" t="s">
         <v>100</v>
       </c>
+      <c r="I157" s="1" t="s">
+        <v>748</v>
+      </c>
       <c r="J157" s="1" t="s">
         <v>13</v>
       </c>
@@ -9017,6 +9671,9 @@
       <c r="H158" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="I158" s="1" t="s">
+        <v>685</v>
+      </c>
       <c r="J158" s="1" t="s">
         <v>24</v>
       </c>
@@ -9055,6 +9712,9 @@
       <c r="H159" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="I159" s="1" t="s">
+        <v>749</v>
+      </c>
       <c r="J159" s="1" t="s">
         <v>6</v>
       </c>
@@ -9093,6 +9753,9 @@
       <c r="H160" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="I160" s="1" t="s">
+        <v>685</v>
+      </c>
       <c r="J160" s="1" t="s">
         <v>24</v>
       </c>
@@ -9131,6 +9794,9 @@
       <c r="H161" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="I161" s="1" t="s">
+        <v>750</v>
+      </c>
       <c r="J161" s="1" t="s">
         <v>75</v>
       </c>
@@ -9169,6 +9835,9 @@
       <c r="H162" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="I162" s="1" t="s">
+        <v>699</v>
+      </c>
       <c r="J162" s="1" t="s">
         <v>13</v>
       </c>
@@ -9207,6 +9876,9 @@
       <c r="H163" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I163" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J163" s="1" t="s">
         <v>6</v>
       </c>
@@ -9245,6 +9917,9 @@
       <c r="H164" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I164" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J164" s="1" t="s">
         <v>6</v>
       </c>
@@ -9283,6 +9958,9 @@
       <c r="H165" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="I165" s="1" t="s">
+        <v>699</v>
+      </c>
       <c r="J165" s="1" t="s">
         <v>13</v>
       </c>
@@ -9321,6 +9999,9 @@
       <c r="H166" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="I166" s="1" t="s">
+        <v>687</v>
+      </c>
       <c r="J166" s="1" t="s">
         <v>2</v>
       </c>
@@ -9359,6 +10040,9 @@
       <c r="H167" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="I167" s="1" t="s">
+        <v>697</v>
+      </c>
       <c r="J167" s="1" t="s">
         <v>71</v>
       </c>
@@ -9397,6 +10081,9 @@
       <c r="H168" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="I168" s="1" t="s">
+        <v>686</v>
+      </c>
       <c r="J168" s="1" t="s">
         <v>42</v>
       </c>
@@ -9435,6 +10122,9 @@
       <c r="H169" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="I169" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J169" s="1" t="s">
         <v>6</v>
       </c>
@@ -9473,6 +10163,9 @@
       <c r="H170" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="I170" s="1" t="s">
+        <v>694</v>
+      </c>
       <c r="J170" s="1" t="s">
         <v>13</v>
       </c>
@@ -9511,6 +10204,9 @@
       <c r="H171" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="I171" s="1" t="s">
+        <v>694</v>
+      </c>
       <c r="J171" s="1" t="s">
         <v>13</v>
       </c>
@@ -9549,6 +10245,9 @@
       <c r="H172" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="I172" s="1" t="s">
+        <v>751</v>
+      </c>
       <c r="J172" s="1" t="s">
         <v>2</v>
       </c>
@@ -9587,6 +10286,9 @@
       <c r="H173" s="1" t="s">
         <v>358</v>
       </c>
+      <c r="I173" s="1" t="s">
+        <v>752</v>
+      </c>
       <c r="J173" s="1" t="s">
         <v>42</v>
       </c>
@@ -9625,6 +10327,9 @@
       <c r="H174" s="1" t="s">
         <v>343</v>
       </c>
+      <c r="I174" s="1" t="s">
+        <v>753</v>
+      </c>
       <c r="J174" s="1" t="s">
         <v>13</v>
       </c>
@@ -9660,6 +10365,9 @@
       <c r="H175" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I175" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J175" s="1" t="s">
         <v>6</v>
       </c>
@@ -9695,6 +10403,9 @@
       <c r="H176" s="1" t="s">
         <v>337</v>
       </c>
+      <c r="I176" s="1" t="s">
+        <v>754</v>
+      </c>
       <c r="J176" s="1" t="s">
         <v>2</v>
       </c>
@@ -9733,6 +10444,9 @@
       <c r="H177" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I177" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J177" s="1" t="s">
         <v>6</v>
       </c>
@@ -9771,6 +10485,9 @@
       <c r="H178" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I178" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J178" s="1" t="s">
         <v>6</v>
       </c>
@@ -9806,6 +10523,9 @@
       <c r="H179" s="1" t="s">
         <v>340</v>
       </c>
+      <c r="I179" s="1" t="s">
+        <v>340</v>
+      </c>
       <c r="J179" s="1" t="s">
         <v>71</v>
       </c>
@@ -9844,6 +10564,9 @@
       <c r="H180" s="1" t="s">
         <v>348</v>
       </c>
+      <c r="I180" s="1" t="s">
+        <v>755</v>
+      </c>
       <c r="J180" s="1" t="s">
         <v>297</v>
       </c>
@@ -9882,6 +10605,9 @@
       <c r="H181" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I181" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J181" s="1" t="s">
         <v>6</v>
       </c>
@@ -9920,6 +10646,9 @@
       <c r="H182" s="1" t="s">
         <v>137</v>
       </c>
+      <c r="I182" s="1" t="s">
+        <v>756</v>
+      </c>
       <c r="J182" s="1" t="s">
         <v>6</v>
       </c>
@@ -9955,6 +10684,9 @@
       <c r="H183" s="1" t="s">
         <v>347</v>
       </c>
+      <c r="I183" s="1" t="s">
+        <v>757</v>
+      </c>
       <c r="J183" s="1" t="s">
         <v>6</v>
       </c>
@@ -9993,6 +10725,9 @@
       <c r="H184" s="1" t="s">
         <v>350</v>
       </c>
+      <c r="I184" s="1" t="s">
+        <v>758</v>
+      </c>
       <c r="J184" s="1" t="s">
         <v>13</v>
       </c>
@@ -10031,6 +10766,9 @@
       <c r="H185" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I185" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J185" s="1" t="s">
         <v>6</v>
       </c>
@@ -10069,6 +10807,9 @@
       <c r="H186" s="1" t="s">
         <v>357</v>
       </c>
+      <c r="I186" s="1" t="s">
+        <v>759</v>
+      </c>
       <c r="J186" s="1" t="s">
         <v>13</v>
       </c>
@@ -10107,6 +10848,9 @@
       <c r="H187" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I187" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J187" s="1" t="s">
         <v>6</v>
       </c>
@@ -10145,6 +10889,9 @@
       <c r="H188" s="1" t="s">
         <v>354</v>
       </c>
+      <c r="I188" s="1" t="s">
+        <v>760</v>
+      </c>
       <c r="J188" s="1" t="s">
         <v>13</v>
       </c>
@@ -10183,6 +10930,9 @@
       <c r="H189" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="I189" s="1" t="s">
+        <v>340</v>
+      </c>
       <c r="J189" s="1" t="s">
         <v>71</v>
       </c>
@@ -10221,6 +10971,9 @@
       <c r="H190" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I190" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J190" s="1" t="s">
         <v>6</v>
       </c>
@@ -10259,6 +11012,9 @@
       <c r="H191" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I191" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J191" s="1" t="s">
         <v>6</v>
       </c>
@@ -10297,6 +11053,9 @@
       <c r="H192" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I192" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J192" s="1" t="s">
         <v>6</v>
       </c>
@@ -10335,6 +11094,9 @@
       <c r="H193" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="I193" s="1" t="s">
+        <v>746</v>
+      </c>
       <c r="J193" s="1" t="s">
         <v>71</v>
       </c>
@@ -10373,6 +11135,9 @@
       <c r="H194" s="1" t="s">
         <v>300</v>
       </c>
+      <c r="I194" s="1" t="s">
+        <v>761</v>
+      </c>
       <c r="J194" s="1" t="s">
         <v>24</v>
       </c>
@@ -10405,6 +11170,9 @@
       <c r="H195" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I195" s="1" t="s">
+        <v>684</v>
+      </c>
       <c r="J195" s="1" t="s">
         <v>6</v>
       </c>
@@ -10440,6 +11208,9 @@
       <c r="H196" s="1" t="s">
         <v>302</v>
       </c>
+      <c r="I196" s="1" t="s">
+        <v>762</v>
+      </c>
       <c r="J196" s="1" t="s">
         <v>13</v>
       </c>
@@ -10472,6 +11243,9 @@
       <c r="H197" s="1" t="s">
         <v>272</v>
       </c>
+      <c r="I197" s="1" t="s">
+        <v>763</v>
+      </c>
       <c r="J197" s="1" t="s">
         <v>6</v>
       </c>
@@ -10504,6 +11278,9 @@
       <c r="H198" s="1" t="s">
         <v>349</v>
       </c>
+      <c r="I198" s="1" t="s">
+        <v>349</v>
+      </c>
       <c r="J198" s="1" t="s">
         <v>306</v>
       </c>
@@ -10536,6 +11313,9 @@
       <c r="H199" s="1" t="s">
         <v>356</v>
       </c>
+      <c r="I199" s="1" t="s">
+        <v>764</v>
+      </c>
       <c r="J199" s="1" t="s">
         <v>306</v>
       </c>
@@ -10568,6 +11348,9 @@
       <c r="H200" s="1" t="s">
         <v>351</v>
       </c>
+      <c r="I200" s="1" t="s">
+        <v>765</v>
+      </c>
       <c r="J200" s="1" t="s">
         <v>306</v>
       </c>
@@ -10600,6 +11383,9 @@
       <c r="H201" s="1" t="s">
         <v>300</v>
       </c>
+      <c r="I201" s="1" t="s">
+        <v>761</v>
+      </c>
       <c r="J201" s="1" t="s">
         <v>24</v>
       </c>
@@ -10632,6 +11418,9 @@
       <c r="H202" s="1" t="s">
         <v>304</v>
       </c>
+      <c r="I202" s="1" t="s">
+        <v>766</v>
+      </c>
       <c r="J202" s="1" t="s">
         <v>2</v>
       </c>
@@ -10664,6 +11453,9 @@
       <c r="H203" s="1" t="s">
         <v>314</v>
       </c>
+      <c r="I203" s="1" t="s">
+        <v>767</v>
+      </c>
       <c r="J203" s="1" t="s">
         <v>71</v>
       </c>
@@ -10696,6 +11488,9 @@
       <c r="H204" s="1" t="s">
         <v>317</v>
       </c>
+      <c r="I204" s="1" t="s">
+        <v>768</v>
+      </c>
       <c r="J204" s="1" t="s">
         <v>71</v>
       </c>
@@ -10704,7 +11499,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:M204">
+  <sortState ref="A2:N204">
     <sortCondition ref="K2:K204"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>